<commit_message>
Added Backend and new docs
</commit_message>
<xml_diff>
--- a/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
+++ b/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Implemented: Express API gateway with Helmet security headers; HTTPS enforcement middleware; Joi request validation (body/query/params); consistent error shape {code,message,details?} for 400/401/403/404/415/429/500; health check GET /health; request ID (X-Request-Id) on all responses; CORS; JSON-only enforcement; 404 handler; central error handler; business layer stubs (no DB/business logic in API layer). Auth routes wired with validation to business delegation. Node.js/Express stack per architecture section 4.</t>
+          <t>REBUILT on NestJS+TypeScript (locked stack). Modular: /modules/{auth,student,attendance,activities} with controller/service/repository/policy pattern. Global: Helmet; HTTPS enforce; CORS; JSON-only; class-validator DTO pipes; GlobalExceptionFilter; RequestId; Logging; ThrottlerGuard; AuthGuard; AuthorizationGuard; AuditService. Health: GET /health. Auth: POST /v1/auth/* with DTO validation. OpenAPI/Swagger at /api/docs. Zero TS build errors.</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -680,6 +690,11 @@
       <c r="O3" t="inlineStr">
         <is>
           <t>Backlog § Task 1.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>POST /v1/auth/mpin/verify: bcrypt MPIN hash via AuthRepository (in-memory; DB Task 2.1). Success: JWT (1h, studentId). Failure: 401 generic. Lockout: 5 attempts -&gt; 15 min (403). Rate limit: 10/60s. Audit: LOGIN_SUCCESS/FAILURE/LOCKOUT. No MPIN in logs/response.</t>
         </is>
       </c>
     </row>
@@ -732,7 +747,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -743,6 +768,11 @@
       <c r="O4" t="inlineStr">
         <is>
           <t>Backlog § Task 1.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>POST /v1/auth/lockout/status: fully implemented — returns isLocked, lockedUntil, attemptsRemaining, maxAttempts (5), lockoutDurationMinutes (15). POST /v1/auth/forgot-mpin: returns 202 Accepted — v1 entry point; full OTP deferred. Audit logged. Error shape consistent.</t>
         </is>
       </c>
     </row>
@@ -795,7 +825,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -806,6 +846,11 @@
       <c r="O5" t="inlineStr">
         <is>
           <t>Backlog § Task 1.4 Checklist</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>AuthGuard verifies JWT via JwtService.verifyAsync. Expired → 401 TOKEN_EXPIRED; invalid → 401 INVALID_TOKEN; missing → 401 UNAUTHORIZED. Extracts studentId from JWT payload → request.student. @Student() decorator. @Public() bypass. GET /v1/student/me protected demo endpoint. No cross-student access.</t>
         </is>
       </c>
     </row>
@@ -2593,13 +2638,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f>E2-F2</f>

</xml_diff>

<commit_message>
New Sprint Files and Documentationadded
</commit_message>
<xml_diff>
--- a/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
+++ b/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
@@ -903,7 +903,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -914,6 +924,11 @@
       <c r="O6" t="inlineStr">
         <is>
           <t>Backlog § Task 2.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>TypeORM + PostgreSQL (prod) / better-sqlite3 (dev). 11 entities per §5.1. Indexes on student_id, activity_id, date, syllabus. Versioned migration (idempotent). DatabaseModule with ConfigService.</t>
         </is>
       </c>
     </row>
@@ -966,7 +981,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -977,6 +1002,11 @@
       <c r="O7" t="inlineStr">
         <is>
           <t>Backlog § Task 2.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>10 repositories with BaseRepository error handling: retry 3x for transient errors, 409 for duplicates. All queries parameterized and scoped by student_id. AuthRepository migrated to TypeORM. AuditService persists to DB.</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1059,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1040,6 +1080,11 @@
       <c r="O8" t="inlineStr">
         <is>
           <t>Backlog § Task 2.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Business services: StudentService, ActivitiesService, GradingService, AttendanceService, DoubtService. Domain exceptions mapped to HTTP codes. API→Service→Repo layering enforced.</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1137,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1103,6 +1158,11 @@
       <c r="O9" t="inlineStr">
         <is>
           <t>Backlog § Task 3.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>GET /v1/student/today: student context + task cards (id, type, title, syllabusRef, questionCount, estimatedMinutes, status, score) + progress. Auth+student_id scoped. Empty state: empty tasks, 0%. GET /v1/student/profile: profile + totalActivitiesCompleted. DevSeederService seeds 3 activities+5 questions+10 attendance in dev. Coding standards applied.</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1215,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1166,6 +1236,11 @@
       <c r="O10" t="inlineStr">
         <is>
           <t>Backlog § Task 3.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>GET /v1/student/activities/:type/:id: metadata + questions (correct answer never exposed). PENDING→IN_PROGRESS on first open. POST pause: marks PAUSED, no-op if completed. Types: homework, quiz, test, gap_bridge. 404 if not assigned.</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1293,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1229,6 +1314,11 @@
       <c r="O11" t="inlineStr">
         <is>
           <t>Backlog § Task 3.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>POST /v1/student/activities/:type/:id/respond: {questionId, answer, requestFeedbackLevel?}. Deterministic grading MCQ/TF/FILL_BLANK. Returns isCorrect, score, feedback, feedbackLevel, isComplete, nextQuestionId. Idempotent duplicate submit. Auto-completes on all answered. 409 if completed.</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1371,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1292,6 +1392,11 @@
       <c r="O12" t="inlineStr">
         <is>
           <t>Backlog § Task 3.4 Checklist</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>GET /v1/student/results/:type/:id: score, breakdown[{questionId,isCorrect,score}], suggestedNext[{type,title,reason}]. Suggested: &lt;60%→gap_bridge, 60-89%→quiz, 90%+→next topic. 404 if not found.</t>
         </is>
       </c>
     </row>
@@ -2664,7 +2769,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>3</v>
@@ -2687,13 +2792,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
New Sprint Files and Documentation added
</commit_message>
<xml_diff>
--- a/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
+++ b/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
@@ -1449,7 +1449,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1460,6 +1470,11 @@
       <c r="O13" t="inlineStr">
         <is>
           <t>Backlog § Task 4.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>AiProviderService: OpenAI-compatible HTTP via native fetch+AbortController. 10s timeout→deterministic fallback. Response validated. Token usage logged. PromptBuilderService: grading/feedback/doubt prompts (no PII). Cost tiering: grading=cheap, feedback=higher. AiModule @Global. Config: AI_BASE_URL/API_KEY/MODELS/TIMEOUT/MAX_TOKENS/TEMPERATURE.</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1527,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1523,6 +1548,11 @@
       <c r="O14" t="inlineStr">
         <is>
           <t>Backlog § Task 4.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>GET /v1/student/activities/:type/:id/feedback?questionId=&amp;level=. FeedbackService: Hint→Approach→Concept→Solution. Auto-advances, monotonic progression enforced. Returns {questionId,level,content,fromAi,nextLevel,maxLevelReached}. Persists feedbackLevel+aiFeedback to response. Static fallback when AI unavailable.</t>
         </is>
       </c>
     </row>
@@ -1575,7 +1605,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1586,6 +1626,11 @@
       <c r="O15" t="inlineStr">
         <is>
           <t>Backlog § Task 4.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>GradingService: MCQ/TF/FILL_BLANK→deterministic (case-insensitive, 0/100). SHORT/LONG_ANSWER→AI-assisted with rubric; JSON response parsed. No API key→pending. ActivitiesService delegates to GradingService. AI results stored in response entity. No PII in prompts.</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1683,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1649,6 +1704,11 @@
       <c r="O16" t="inlineStr">
         <is>
           <t>Backlog § Task 5.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>GET /v1/student/attendance: AttendanceController + AttendanceQueryDto with period shortcuts (this_month, last_month, this_term) or explicit dates. Summary + calendar. Timezone-safe. Auth + scoped. Validation.</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1761,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1712,6 +1782,11 @@
       <c r="O17" t="inlineStr">
         <is>
           <t>Backlog § Task 5.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>DoubtsController: GET list + GET thread + POST message with syllabus context. SyllabusController: GET /v1/student/syllabus/tree. Replies inherit thread syllabus context. AI fallback. Full DTO validation.</t>
         </is>
       </c>
     </row>
@@ -1764,7 +1839,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1775,6 +1860,11 @@
       <c r="O18" t="inlineStr">
         <is>
           <t>Backlog § Task 5.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Enhanced profile with progressOverview (activity breakdown by type with avg scores). GET /v1/student/sync/status with conflict hint (stub - real sync Sprint 7).</t>
         </is>
       </c>
     </row>
@@ -2743,13 +2833,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <f>E2-F2</f>
@@ -2769,13 +2859,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
         <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f>E3-F3</f>
@@ -2795,13 +2885,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <f>E4-F4</f>
@@ -2827,7 +2917,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f>E5-F5</f>
@@ -2853,7 +2943,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <f>E6-F6</f>

</xml_diff>

<commit_message>
added new docs and frontend codes
</commit_message>
<xml_diff>
--- a/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
+++ b/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
@@ -140,6 +140,454 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Overall Task Completion</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sprint Summary'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <dPt>
+            <idx val="0"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="4CAF50"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="1"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="E0E0E0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dLbls>
+            <showVal val="1"/>
+            <showCatName val="1"/>
+            <showPercent val="1"/>
+          </dLbls>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$I$2:$I$3</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$J$2:$J$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Sprint Progress (Tasks Done vs Total)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sprint Summary'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="BDBDBD"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$B$2:$B$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Sprint Summary'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="4CAF50"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <dLbls>
+            <showVal val="1"/>
+          </dLbls>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$B$2:$B$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$F$2:$F$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Story Points: Planned vs Delivered</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sprint Summary'!M1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="90CAF9"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$L$2:$L$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$M$2:$M$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Sprint Summary'!N1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="1565C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <dLbls>
+            <showVal val="1"/>
+          </dLbls>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$L$2:$L$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$N$2:$N$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Story Points</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5760000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7920000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>37</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7920000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1917,7 +2365,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1928,6 +2386,11 @@
       <c r="O19" t="inlineStr">
         <is>
           <t>Backlog § Task 6.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>React+TS+Vite client. API client with Bearer auth, error parsing, retry/timeout. AuthContext + sessionStorage. Vite proxy. Design tokens. BottomNav + Skeleton.</t>
         </is>
       </c>
     </row>
@@ -1980,7 +2443,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -1991,6 +2464,11 @@
       <c r="O20" t="inlineStr">
         <is>
           <t>Backlog § Task 6.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Login: 6-digit MPIN dots + keypad. Auto-submit. States: default, entering, loading, error (attempts), locked (countdown). Accessibility.</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2521,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2054,6 +2542,11 @@
       <c r="O21" t="inlineStr">
         <is>
           <t>Backlog § Task 6.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Home: greeting, progress bar, task cards (type/status/title/subject/questions/time). States: loading, default, empty, error. BottomNav.</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2599,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2117,6 +2620,11 @@
       <c r="O22" t="inlineStr">
         <is>
           <t>Backlog § Task 6.4 Checklist</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Activity: question flow with MCQ options or text input. Submit → correct/incorrect + AI feedback panel (progressive hints). Pause saves progress.</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2677,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2180,6 +2698,11 @@
       <c r="O23" t="inlineStr">
         <is>
           <t>Backlog § Task 6.5 Checklist</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Results: score circle, star rating, per-question breakdown, suggested next, Back to Home. Perfect score celebration.</t>
         </is>
       </c>
     </row>
@@ -2766,7 +3289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2819,6 +3342,31 @@
           <t>Remaining</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Sprint</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Planned SP</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Delivered SP</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2845,6 +3393,25 @@
         <f>E2-F2</f>
         <v/>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Completed (22)</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>22</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Foundation &amp; Auth</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>8</v>
+      </c>
+      <c r="N2" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -2871,6 +3438,25 @@
         <f>E3-F3</f>
         <v/>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Remaining (9)</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Data &amp; Backend Core</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2897,6 +3483,17 @@
         <f>E4-F4</f>
         <v/>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Today's Plan &amp; Activities API</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>8</v>
+      </c>
+      <c r="N4" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -2923,6 +3520,17 @@
         <f>E5-F5</f>
         <v/>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>AI Integration &amp; Grading</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>8</v>
+      </c>
+      <c r="N5" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -2949,6 +3557,17 @@
         <f>E6-F6</f>
         <v/>
       </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Attendance &amp; Doubts API</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>7</v>
+      </c>
+      <c r="N6" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -2969,12 +3588,23 @@
         <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f>E7-F7</f>
         <v/>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Client — Login, Home, Activity, Results</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3001,6 +3631,17 @@
         <f>E8-F8</f>
         <v/>
       </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Client — Attendance, Doubts, Profile &amp; Sync</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -3027,8 +3668,20 @@
         <f>E9-F9</f>
         <v/>
       </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>DevOps, Security Hardening &amp; NotebookLM</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>8</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some changes in code and also new screens are added
</commit_message>
<xml_diff>
--- a/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
+++ b/docs/planning/Mindforge_Student_Experience_Project_Tracking.xlsx
@@ -144,7 +144,6 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -177,33 +176,6 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <dPt>
-            <idx val="0"/>
-            <spPr>
-              <a:solidFill>
-                <a:srgbClr val="4CAF50"/>
-              </a:solidFill>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dPt>
-            <idx val="1"/>
-            <spPr>
-              <a:solidFill>
-                <a:srgbClr val="E0E0E0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dLbls>
-            <showVal val="1"/>
-            <showCatName val="1"/>
-            <showPercent val="1"/>
-          </dLbls>
           <cat>
             <numRef>
               <f>'Sprint Summary'!$I$2:$I$3</f>
@@ -229,7 +201,6 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -255,13 +226,34 @@
           <order val="0"/>
           <tx>
             <strRef>
+              <f>'Sprint Summary'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sprint Summary'!$B$2:$B$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sprint Summary'!$F$2:$F$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
               <f>'Sprint Summary'!E1</f>
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
-              <a:srgbClr val="BDBDBD"/>
-            </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -277,36 +269,6 @@
             </numRef>
           </val>
         </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Sprint Summary'!F1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4CAF50"/>
-            </a:solidFill>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <dLbls>
-            <showVal val="1"/>
-          </dLbls>
-          <cat>
-            <numRef>
-              <f>'Sprint Summary'!$B$2:$B$9</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Sprint Summary'!$F$2:$F$9</f>
-            </numRef>
-          </val>
-        </ser>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
@@ -317,21 +279,6 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Sprint</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -353,7 +300,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Number of Tasks</a:t>
+                  <a:t>Tasks</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -375,7 +322,6 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -405,9 +351,6 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
-              <a:srgbClr val="90CAF9"/>
-            </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -432,16 +375,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
-              <a:srgbClr val="1565C0"/>
-            </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <dLbls>
-            <showVal val="1"/>
-          </dLbls>
           <cat>
             <numRef>
               <f>'Sprint Summary'!$L$2:$L$9</f>
@@ -463,21 +400,6 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Sprint</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -523,12 +445,12 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>8</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>5</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5760000" cy="4320000"/>
+    <ext cx="5400000" cy="2700000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -545,12 +467,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>8</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>21</row>
+      <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7920000" cy="4320000"/>
+    <ext cx="5400000" cy="2700000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -567,12 +489,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>8</col>
+      <col>15</col>
       <colOff>0</colOff>
-      <row>37</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7920000" cy="4320000"/>
+    <ext cx="5400000" cy="2700000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="3" name="Chart 3"/>
@@ -2755,7 +2677,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2766,6 +2698,11 @@
       <c r="O24" t="inlineStr">
         <is>
           <t>Backlog § Task 7.1 Checklist</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Route /attendance. Period selector, summary card (Present/Absent/Late/Rate), calendar grid with coloured day dots, legend. Loading/empty/error states. Timezone-safe. SVG icons in bottom nav.</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2755,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2829,6 +2776,11 @@
       <c r="O25" t="inlineStr">
         <is>
           <t>Backlog § Task 7.2 Checklist</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Route /doubts. Thread list + chat. Syllabus context bar with cascading Subject→Chapter→Topic picker. Student/AI chat bubbles, auto-scroll, thinking indicator. Context inheritance on replies.</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2833,17 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2892,6 +2854,11 @@
       <c r="O26" t="inlineStr">
         <is>
           <t>Backlog § Task 7.3 Checklist</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Route /profile. Avatar initial, name, Class/Board chips. Progress overview per activity type with mini bars. Quick links to Attendance/Doubts. Logout with confirmation dialog.</t>
         </is>
       </c>
     </row>
@@ -2944,7 +2911,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2955,6 +2932,11 @@
       <c r="O27" t="inlineStr">
         <is>
           <t>Backlog § Task 7.4 Checklist</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>SyncBanner on HomeScreen. Polls sync/status every 60s. Green/orange dot. Conflict modal with Keep Current / Use Latest actions.</t>
         </is>
       </c>
     </row>
@@ -3395,11 +3377,11 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Completed (22)</t>
+          <t>Completed (26)</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -3440,11 +3422,11 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Remaining (9)</t>
+          <t>Remaining (5)</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -3625,7 +3607,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f>E8-F8</f>
@@ -3640,7 +3622,7 @@
         <v>8</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">

</xml_diff>